<commit_message>
changes the script for buyAMC on 16-02-2023
</commit_message>
<xml_diff>
--- a/Auto_EFL/EFL/src/test/resources/testdata/testfile.xlsx
+++ b/Auto_EFL/EFL/src/test/resources/testdata/testfile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15915" windowHeight="7695" firstSheet="3" activeTab="5"/>
+    <workbookView windowWidth="15900" windowHeight="7695" firstSheet="4" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Selectcategory" sheetId="3" r:id="rId1"/>
@@ -15,13 +15,14 @@
     <sheet name="BuyAmc" sheetId="12" r:id="rId6"/>
     <sheet name="Demo" sheetId="14" r:id="rId7"/>
     <sheet name="LoginCheckout" sheetId="15" r:id="rId8"/>
+    <sheet name="1" sheetId="16" r:id="rId9"/>
   </sheets>
   <calcPr calcId="144525" iterate="1" iterateCount="100" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="58">
   <si>
     <t>WayToClickOnMenu</t>
   </si>
@@ -176,7 +177,19 @@
     <t>ChoosePlan</t>
   </si>
   <si>
+    <t>ChoosePlanHome</t>
+  </si>
+  <si>
+    <t>ChoosePlanProfile</t>
+  </si>
+  <si>
     <t>1-year plan</t>
+  </si>
+  <si>
+    <t>2-year plan</t>
+  </si>
+  <si>
+    <t>3-year plan</t>
   </si>
   <si>
     <t>Water1</t>
@@ -190,12 +203,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="26">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -222,6 +235,12 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF343A40"/>
+      <name val="Neue-Haas-Unica-W01-Medium"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="9"/>
       <color rgb="FF343A40"/>
       <name val="Neue-Haas-Unica-W01-Medium"/>
@@ -235,16 +254,61 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -255,6 +319,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -262,8 +366,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -277,57 +382,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -339,43 +395,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -392,115 +411,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -512,67 +591,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -619,21 +638,6 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -686,6 +690,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -714,152 +733,152 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -872,9 +891,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1262,13 +1282,13 @@
       <c r="A3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="14" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="15" t="s">
         <v>16</v>
       </c>
       <c r="E3" s="11" t="s">
@@ -1522,7 +1542,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1546,25 +1566,39 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="19.1428571428571" customWidth="1"/>
+    <col min="2" max="2" width="17.5714285714286" customWidth="1"/>
+    <col min="3" max="3" width="18.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" ht="15" spans="1:3">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1617,7 +1651,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="9" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>8</v>
@@ -1705,7 +1739,7 @@
     </row>
     <row r="2" ht="15" spans="1:14">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B2">
         <v>8899767878</v>
@@ -1754,4 +1788,20 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>